<commit_message>
FDR correction of p-values of Spearman and Pearson test
</commit_message>
<xml_diff>
--- a/labels_data.xlsx
+++ b/labels_data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="List1" sheetId="1" r:id="rId1"/>
@@ -2719,15 +2719,15 @@
   <dimension ref="A1:J520"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+      <selection activeCell="P8" sqref="P8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="10" width="16.21875" style="31" customWidth="1"/>
+    <col min="1" max="10" width="16.28515625" style="31" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2759,7 +2759,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>9</v>
       </c>
@@ -2781,7 +2781,7 @@
       <c r="I2" s="6"/>
       <c r="J2" s="7"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>13</v>
       </c>
@@ -2803,7 +2803,7 @@
       <c r="I3" s="6"/>
       <c r="J3" s="7"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>15</v>
       </c>
@@ -2825,7 +2825,7 @@
       <c r="I4" s="6"/>
       <c r="J4" s="7"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>16</v>
       </c>
@@ -2847,7 +2847,7 @@
       <c r="I5" s="6"/>
       <c r="J5" s="7"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>17</v>
       </c>
@@ -2869,7 +2869,7 @@
       <c r="I6" s="6"/>
       <c r="J6" s="7"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>18</v>
       </c>
@@ -2891,7 +2891,7 @@
       <c r="I7" s="6"/>
       <c r="J7" s="7"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>19</v>
       </c>
@@ -2913,7 +2913,7 @@
       <c r="I8" s="6"/>
       <c r="J8" s="7"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>20</v>
       </c>
@@ -2935,7 +2935,7 @@
       <c r="I9" s="6"/>
       <c r="J9" s="7"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>21</v>
       </c>
@@ -2957,7 +2957,7 @@
       <c r="I10" s="6"/>
       <c r="J10" s="7"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>22</v>
       </c>
@@ -2979,7 +2979,7 @@
       <c r="I11" s="6"/>
       <c r="J11" s="7"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>23</v>
       </c>
@@ -3001,7 +3001,7 @@
       <c r="I12" s="6"/>
       <c r="J12" s="7"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>24</v>
       </c>
@@ -3023,7 +3023,7 @@
       <c r="I13" s="6"/>
       <c r="J13" s="7"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>25</v>
       </c>
@@ -3045,7 +3045,7 @@
       <c r="I14" s="6"/>
       <c r="J14" s="7"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>26</v>
       </c>
@@ -3067,7 +3067,7 @@
       <c r="I15" s="6"/>
       <c r="J15" s="7"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>27</v>
       </c>
@@ -3089,7 +3089,7 @@
       <c r="I16" s="6"/>
       <c r="J16" s="7"/>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>28</v>
       </c>
@@ -3111,7 +3111,7 @@
       <c r="I17" s="6"/>
       <c r="J17" s="7"/>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>29</v>
       </c>
@@ -3133,7 +3133,7 @@
       <c r="I18" s="6"/>
       <c r="J18" s="7"/>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>30</v>
       </c>
@@ -3155,7 +3155,7 @@
       <c r="I19" s="6"/>
       <c r="J19" s="7"/>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
         <v>31</v>
       </c>
@@ -3177,7 +3177,7 @@
       <c r="I20" s="6"/>
       <c r="J20" s="7"/>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>32</v>
       </c>
@@ -3199,7 +3199,7 @@
       <c r="I21" s="6"/>
       <c r="J21" s="7"/>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
         <v>33</v>
       </c>
@@ -3221,7 +3221,7 @@
       <c r="I22" s="6"/>
       <c r="J22" s="7"/>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>34</v>
       </c>
@@ -3243,7 +3243,7 @@
       <c r="I23" s="6"/>
       <c r="J23" s="7"/>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
         <v>35</v>
       </c>
@@ -3265,7 +3265,7 @@
       <c r="I24" s="6"/>
       <c r="J24" s="7"/>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
         <v>36</v>
       </c>
@@ -3287,7 +3287,7 @@
       <c r="I25" s="6"/>
       <c r="J25" s="7"/>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
         <v>37</v>
       </c>
@@ -3309,7 +3309,7 @@
       <c r="I26" s="6"/>
       <c r="J26" s="7"/>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
         <v>38</v>
       </c>
@@ -3331,7 +3331,7 @@
       <c r="I27" s="6"/>
       <c r="J27" s="7"/>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
         <v>39</v>
       </c>
@@ -3353,7 +3353,7 @@
       <c r="I28" s="6"/>
       <c r="J28" s="7"/>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
         <v>40</v>
       </c>
@@ -3375,7 +3375,7 @@
       <c r="I29" s="6"/>
       <c r="J29" s="7"/>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
         <v>41</v>
       </c>
@@ -3397,7 +3397,7 @@
       <c r="I30" s="6"/>
       <c r="J30" s="7"/>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
         <v>42</v>
       </c>
@@ -3419,7 +3419,7 @@
       <c r="I31" s="6"/>
       <c r="J31" s="7"/>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
         <v>43</v>
       </c>
@@ -3447,7 +3447,7 @@
       <c r="I32" s="6"/>
       <c r="J32" s="7"/>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
         <v>45</v>
       </c>
@@ -3475,7 +3475,7 @@
       <c r="I33" s="6"/>
       <c r="J33" s="7"/>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
         <v>46</v>
       </c>
@@ -3503,7 +3503,7 @@
       <c r="I34" s="6"/>
       <c r="J34" s="7"/>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
         <v>47</v>
       </c>
@@ -3531,7 +3531,7 @@
       <c r="I35" s="6"/>
       <c r="J35" s="7"/>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
         <v>48</v>
       </c>
@@ -3559,7 +3559,7 @@
       <c r="I36" s="6"/>
       <c r="J36" s="7"/>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
         <v>49</v>
       </c>
@@ -3587,7 +3587,7 @@
       <c r="I37" s="6"/>
       <c r="J37" s="7"/>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
         <v>50</v>
       </c>
@@ -3615,7 +3615,7 @@
       <c r="I38" s="6"/>
       <c r="J38" s="7"/>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
         <v>51</v>
       </c>
@@ -3643,7 +3643,7 @@
       <c r="I39" s="6"/>
       <c r="J39" s="7"/>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
         <v>52</v>
       </c>
@@ -3671,7 +3671,7 @@
       <c r="I40" s="6"/>
       <c r="J40" s="7"/>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
         <v>53</v>
       </c>
@@ -3699,7 +3699,7 @@
       <c r="I41" s="6"/>
       <c r="J41" s="7"/>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
         <v>54</v>
       </c>
@@ -3727,7 +3727,7 @@
       <c r="I42" s="6"/>
       <c r="J42" s="7"/>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
         <v>55</v>
       </c>
@@ -3755,7 +3755,7 @@
       <c r="I43" s="6"/>
       <c r="J43" s="7"/>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
         <v>56</v>
       </c>
@@ -3783,7 +3783,7 @@
       <c r="I44" s="6"/>
       <c r="J44" s="7"/>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
         <v>57</v>
       </c>
@@ -3811,7 +3811,7 @@
       <c r="I45" s="6"/>
       <c r="J45" s="7"/>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
         <v>58</v>
       </c>
@@ -3839,7 +3839,7 @@
       <c r="I46" s="6"/>
       <c r="J46" s="7"/>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
         <v>59</v>
       </c>
@@ -3867,7 +3867,7 @@
       <c r="I47" s="6"/>
       <c r="J47" s="7"/>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" s="4" t="s">
         <v>60</v>
       </c>
@@ -3895,7 +3895,7 @@
       <c r="I48" s="6"/>
       <c r="J48" s="7"/>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="s">
         <v>61</v>
       </c>
@@ -3923,7 +3923,7 @@
       <c r="I49" s="6"/>
       <c r="J49" s="7"/>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="s">
         <v>62</v>
       </c>
@@ -3951,7 +3951,7 @@
       <c r="I50" s="6"/>
       <c r="J50" s="7"/>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
         <v>63</v>
       </c>
@@ -3979,7 +3979,7 @@
       <c r="I51" s="6"/>
       <c r="J51" s="7"/>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" s="4" t="s">
         <v>64</v>
       </c>
@@ -4007,7 +4007,7 @@
       <c r="I52" s="6"/>
       <c r="J52" s="7"/>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="s">
         <v>65</v>
       </c>
@@ -4035,7 +4035,7 @@
       <c r="I53" s="6"/>
       <c r="J53" s="7"/>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="s">
         <v>66</v>
       </c>
@@ -4063,7 +4063,7 @@
       <c r="I54" s="6"/>
       <c r="J54" s="7"/>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="s">
         <v>67</v>
       </c>
@@ -4091,7 +4091,7 @@
       <c r="I55" s="6"/>
       <c r="J55" s="7"/>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" s="4" t="s">
         <v>68</v>
       </c>
@@ -4119,7 +4119,7 @@
       <c r="I56" s="6"/>
       <c r="J56" s="7"/>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" s="4" t="s">
         <v>69</v>
       </c>
@@ -4147,7 +4147,7 @@
       <c r="I57" s="6"/>
       <c r="J57" s="7"/>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" s="4" t="s">
         <v>70</v>
       </c>
@@ -4175,7 +4175,7 @@
       <c r="I58" s="6"/>
       <c r="J58" s="7"/>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" s="4" t="s">
         <v>71</v>
       </c>
@@ -4203,7 +4203,7 @@
       <c r="I59" s="6"/>
       <c r="J59" s="7"/>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" s="4" t="s">
         <v>72</v>
       </c>
@@ -4231,7 +4231,7 @@
       <c r="I60" s="6"/>
       <c r="J60" s="7"/>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" s="4" t="s">
         <v>73</v>
       </c>
@@ -4259,7 +4259,7 @@
       <c r="I61" s="6"/>
       <c r="J61" s="7"/>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62" s="4" t="s">
         <v>74</v>
       </c>
@@ -4287,7 +4287,7 @@
       <c r="I62" s="6"/>
       <c r="J62" s="7"/>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" s="4" t="s">
         <v>75</v>
       </c>
@@ -4315,7 +4315,7 @@
       <c r="I63" s="6"/>
       <c r="J63" s="7"/>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64" s="4" t="s">
         <v>76</v>
       </c>
@@ -4343,7 +4343,7 @@
       <c r="I64" s="6"/>
       <c r="J64" s="7"/>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65" s="4" t="s">
         <v>77</v>
       </c>
@@ -4365,7 +4365,7 @@
       <c r="I65" s="6"/>
       <c r="J65" s="7"/>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66" s="4" t="s">
         <v>78</v>
       </c>
@@ -4387,7 +4387,7 @@
       <c r="I66" s="6"/>
       <c r="J66" s="7"/>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67" s="4" t="s">
         <v>79</v>
       </c>
@@ -4409,7 +4409,7 @@
       <c r="I67" s="6"/>
       <c r="J67" s="7"/>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68" s="4" t="s">
         <v>80</v>
       </c>
@@ -4431,7 +4431,7 @@
       <c r="I68" s="6"/>
       <c r="J68" s="7"/>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69" s="4" t="s">
         <v>81</v>
       </c>
@@ -4453,7 +4453,7 @@
       <c r="I69" s="6"/>
       <c r="J69" s="7"/>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70" s="4" t="s">
         <v>82</v>
       </c>
@@ -4475,7 +4475,7 @@
       <c r="I70" s="6"/>
       <c r="J70" s="7"/>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71" s="4" t="s">
         <v>83</v>
       </c>
@@ -4497,7 +4497,7 @@
       <c r="I71" s="6"/>
       <c r="J71" s="7"/>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72" s="4" t="s">
         <v>84</v>
       </c>
@@ -4519,7 +4519,7 @@
       <c r="I72" s="6"/>
       <c r="J72" s="7"/>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A73" s="4" t="s">
         <v>85</v>
       </c>
@@ -4541,7 +4541,7 @@
       <c r="I73" s="6"/>
       <c r="J73" s="7"/>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A74" s="4" t="s">
         <v>86</v>
       </c>
@@ -4563,7 +4563,7 @@
       <c r="I74" s="6"/>
       <c r="J74" s="7"/>
     </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A75" s="4" t="s">
         <v>87</v>
       </c>
@@ -4585,7 +4585,7 @@
       <c r="I75" s="6"/>
       <c r="J75" s="7"/>
     </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A76" s="4" t="s">
         <v>88</v>
       </c>
@@ -4607,7 +4607,7 @@
       <c r="I76" s="6"/>
       <c r="J76" s="7"/>
     </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A77" s="4" t="s">
         <v>89</v>
       </c>
@@ -4629,7 +4629,7 @@
       <c r="I77" s="6"/>
       <c r="J77" s="7"/>
     </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A78" s="4" t="s">
         <v>90</v>
       </c>
@@ -4651,7 +4651,7 @@
       <c r="I78" s="6"/>
       <c r="J78" s="7"/>
     </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A79" s="4" t="s">
         <v>91</v>
       </c>
@@ -4673,7 +4673,7 @@
       <c r="I79" s="6"/>
       <c r="J79" s="7"/>
     </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A80" s="4" t="s">
         <v>92</v>
       </c>
@@ -4695,7 +4695,7 @@
       <c r="I80" s="6"/>
       <c r="J80" s="7"/>
     </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A81" s="4" t="s">
         <v>93</v>
       </c>
@@ -4717,7 +4717,7 @@
       <c r="I81" s="6"/>
       <c r="J81" s="7"/>
     </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A82" s="4" t="s">
         <v>94</v>
       </c>
@@ -4739,7 +4739,7 @@
       <c r="I82" s="6"/>
       <c r="J82" s="7"/>
     </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A83" s="4" t="s">
         <v>95</v>
       </c>
@@ -4761,7 +4761,7 @@
       <c r="I83" s="6"/>
       <c r="J83" s="7"/>
     </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A84" s="4" t="s">
         <v>96</v>
       </c>
@@ -4783,7 +4783,7 @@
       <c r="I84" s="6"/>
       <c r="J84" s="7"/>
     </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A85" s="4" t="s">
         <v>97</v>
       </c>
@@ -4805,7 +4805,7 @@
       <c r="I85" s="6"/>
       <c r="J85" s="7"/>
     </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A86" s="4" t="s">
         <v>98</v>
       </c>
@@ -4827,7 +4827,7 @@
       <c r="I86" s="6"/>
       <c r="J86" s="7"/>
     </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A87" s="4" t="s">
         <v>99</v>
       </c>
@@ -4849,7 +4849,7 @@
       <c r="I87" s="6"/>
       <c r="J87" s="7"/>
     </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A88" s="4" t="s">
         <v>100</v>
       </c>
@@ -4871,7 +4871,7 @@
       <c r="I88" s="6"/>
       <c r="J88" s="7"/>
     </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A89" s="4" t="s">
         <v>101</v>
       </c>
@@ -4893,7 +4893,7 @@
       <c r="I89" s="6"/>
       <c r="J89" s="7"/>
     </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A90" s="4" t="s">
         <v>102</v>
       </c>
@@ -4915,7 +4915,7 @@
       <c r="I90" s="6"/>
       <c r="J90" s="7"/>
     </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A91" s="4" t="s">
         <v>103</v>
       </c>
@@ -4937,7 +4937,7 @@
       <c r="I91" s="6"/>
       <c r="J91" s="7"/>
     </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A92" s="4" t="s">
         <v>104</v>
       </c>
@@ -4959,7 +4959,7 @@
       <c r="I92" s="6"/>
       <c r="J92" s="7"/>
     </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A93" s="4" t="s">
         <v>105</v>
       </c>
@@ -4981,7 +4981,7 @@
       <c r="I93" s="6"/>
       <c r="J93" s="7"/>
     </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A94" s="4" t="s">
         <v>106</v>
       </c>
@@ -5003,7 +5003,7 @@
       <c r="I94" s="6"/>
       <c r="J94" s="7"/>
     </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A95" s="4" t="s">
         <v>107</v>
       </c>
@@ -5025,7 +5025,7 @@
       <c r="I95" s="6"/>
       <c r="J95" s="7"/>
     </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A96" s="4" t="s">
         <v>108</v>
       </c>
@@ -5047,7 +5047,7 @@
       <c r="I96" s="6"/>
       <c r="J96" s="7"/>
     </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A97" s="4" t="s">
         <v>109</v>
       </c>
@@ -5069,7 +5069,7 @@
       <c r="I97" s="6"/>
       <c r="J97" s="7"/>
     </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A98" s="4" t="s">
         <v>110</v>
       </c>
@@ -5091,7 +5091,7 @@
       <c r="I98" s="6"/>
       <c r="J98" s="7"/>
     </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A99" s="4" t="s">
         <v>111</v>
       </c>
@@ -5113,7 +5113,7 @@
       <c r="I99" s="6"/>
       <c r="J99" s="7"/>
     </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A100" s="4" t="s">
         <v>112</v>
       </c>
@@ -5135,7 +5135,7 @@
       <c r="I100" s="6"/>
       <c r="J100" s="7"/>
     </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A101" s="4" t="s">
         <v>113</v>
       </c>
@@ -5157,7 +5157,7 @@
       <c r="I101" s="6"/>
       <c r="J101" s="7"/>
     </row>
-    <row r="102" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A102" s="4" t="s">
         <v>114</v>
       </c>
@@ -5179,7 +5179,7 @@
       <c r="I102" s="6"/>
       <c r="J102" s="7"/>
     </row>
-    <row r="103" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A103" s="4" t="s">
         <v>115</v>
       </c>
@@ -5201,7 +5201,7 @@
       <c r="I103" s="6"/>
       <c r="J103" s="7"/>
     </row>
-    <row r="104" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A104" s="4" t="s">
         <v>116</v>
       </c>
@@ -5223,7 +5223,7 @@
       <c r="I104" s="6"/>
       <c r="J104" s="7"/>
     </row>
-    <row r="105" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A105" s="4" t="s">
         <v>117</v>
       </c>
@@ -5245,7 +5245,7 @@
       <c r="I105" s="6"/>
       <c r="J105" s="7"/>
     </row>
-    <row r="106" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A106" s="4" t="s">
         <v>118</v>
       </c>
@@ -5267,7 +5267,7 @@
       <c r="I106" s="6"/>
       <c r="J106" s="7"/>
     </row>
-    <row r="107" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A107" s="4" t="s">
         <v>119</v>
       </c>
@@ -5289,7 +5289,7 @@
       <c r="I107" s="6"/>
       <c r="J107" s="7"/>
     </row>
-    <row r="108" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A108" s="4" t="s">
         <v>120</v>
       </c>
@@ -5311,7 +5311,7 @@
       <c r="I108" s="6"/>
       <c r="J108" s="7"/>
     </row>
-    <row r="109" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A109" s="4" t="s">
         <v>121</v>
       </c>
@@ -5333,7 +5333,7 @@
       <c r="I109" s="6"/>
       <c r="J109" s="7"/>
     </row>
-    <row r="110" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A110" s="4" t="s">
         <v>122</v>
       </c>
@@ -5355,7 +5355,7 @@
       <c r="I110" s="6"/>
       <c r="J110" s="7"/>
     </row>
-    <row r="111" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A111" s="4" t="s">
         <v>123</v>
       </c>
@@ -5377,7 +5377,7 @@
       <c r="I111" s="6"/>
       <c r="J111" s="7"/>
     </row>
-    <row r="112" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A112" s="4" t="s">
         <v>124</v>
       </c>
@@ -5399,7 +5399,7 @@
       <c r="I112" s="6"/>
       <c r="J112" s="7"/>
     </row>
-    <row r="113" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A113" s="4" t="s">
         <v>125</v>
       </c>
@@ -5421,7 +5421,7 @@
       <c r="I113" s="6"/>
       <c r="J113" s="7"/>
     </row>
-    <row r="114" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A114" s="4" t="s">
         <v>126</v>
       </c>
@@ -5443,7 +5443,7 @@
       <c r="I114" s="6"/>
       <c r="J114" s="7"/>
     </row>
-    <row r="115" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A115" s="4" t="s">
         <v>127</v>
       </c>
@@ -5465,7 +5465,7 @@
       <c r="I115" s="6"/>
       <c r="J115" s="7"/>
     </row>
-    <row r="116" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A116" s="4" t="s">
         <v>128</v>
       </c>
@@ -5491,7 +5491,7 @@
       <c r="I116" s="6"/>
       <c r="J116" s="7"/>
     </row>
-    <row r="117" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A117" s="4" t="s">
         <v>129</v>
       </c>
@@ -5517,7 +5517,7 @@
       <c r="I117" s="6"/>
       <c r="J117" s="7"/>
     </row>
-    <row r="118" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A118" s="4" t="s">
         <v>130</v>
       </c>
@@ -5545,7 +5545,7 @@
       <c r="I118" s="6"/>
       <c r="J118" s="7"/>
     </row>
-    <row r="119" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A119" s="4" t="s">
         <v>131</v>
       </c>
@@ -5573,7 +5573,7 @@
       <c r="I119" s="6"/>
       <c r="J119" s="7"/>
     </row>
-    <row r="120" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A120" s="4" t="s">
         <v>132</v>
       </c>
@@ -5601,7 +5601,7 @@
       <c r="I120" s="6"/>
       <c r="J120" s="7"/>
     </row>
-    <row r="121" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A121" s="4" t="s">
         <v>133</v>
       </c>
@@ -5629,7 +5629,7 @@
       <c r="I121" s="6"/>
       <c r="J121" s="7"/>
     </row>
-    <row r="122" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A122" s="4" t="s">
         <v>134</v>
       </c>
@@ -5657,7 +5657,7 @@
       <c r="I122" s="6"/>
       <c r="J122" s="7"/>
     </row>
-    <row r="123" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A123" s="4" t="s">
         <v>135</v>
       </c>
@@ -5685,7 +5685,7 @@
       <c r="I123" s="6"/>
       <c r="J123" s="7"/>
     </row>
-    <row r="124" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A124" s="4" t="s">
         <v>136</v>
       </c>
@@ -5713,7 +5713,7 @@
       <c r="I124" s="6"/>
       <c r="J124" s="7"/>
     </row>
-    <row r="125" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A125" s="4" t="s">
         <v>137</v>
       </c>
@@ -5741,7 +5741,7 @@
       <c r="I125" s="6"/>
       <c r="J125" s="7"/>
     </row>
-    <row r="126" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A126" s="4" t="s">
         <v>138</v>
       </c>
@@ -5769,7 +5769,7 @@
       <c r="I126" s="6"/>
       <c r="J126" s="7"/>
     </row>
-    <row r="127" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A127" s="4" t="s">
         <v>139</v>
       </c>
@@ -5797,7 +5797,7 @@
       <c r="I127" s="6"/>
       <c r="J127" s="7"/>
     </row>
-    <row r="128" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A128" s="4" t="s">
         <v>140</v>
       </c>
@@ -5823,7 +5823,7 @@
       <c r="I128" s="6"/>
       <c r="J128" s="7"/>
     </row>
-    <row r="129" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A129" s="4" t="s">
         <v>141</v>
       </c>
@@ -5849,7 +5849,7 @@
       <c r="I129" s="6"/>
       <c r="J129" s="7"/>
     </row>
-    <row r="130" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A130" s="4" t="s">
         <v>142</v>
       </c>
@@ -5877,7 +5877,7 @@
       <c r="I130" s="6"/>
       <c r="J130" s="7"/>
     </row>
-    <row r="131" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A131" s="4" t="s">
         <v>143</v>
       </c>
@@ -5905,7 +5905,7 @@
       <c r="I131" s="6"/>
       <c r="J131" s="7"/>
     </row>
-    <row r="132" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A132" s="4" t="s">
         <v>144</v>
       </c>
@@ -5933,7 +5933,7 @@
       <c r="I132" s="6"/>
       <c r="J132" s="7"/>
     </row>
-    <row r="133" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A133" s="4" t="s">
         <v>145</v>
       </c>
@@ -5961,7 +5961,7 @@
       <c r="I133" s="6"/>
       <c r="J133" s="7"/>
     </row>
-    <row r="134" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A134" s="4" t="s">
         <v>146</v>
       </c>
@@ -5989,7 +5989,7 @@
       <c r="I134" s="6"/>
       <c r="J134" s="7"/>
     </row>
-    <row r="135" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A135" s="4" t="s">
         <v>147</v>
       </c>
@@ -6017,7 +6017,7 @@
       <c r="I135" s="6"/>
       <c r="J135" s="7"/>
     </row>
-    <row r="136" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A136" s="4" t="s">
         <v>148</v>
       </c>
@@ -6045,7 +6045,7 @@
       <c r="I136" s="6"/>
       <c r="J136" s="7"/>
     </row>
-    <row r="137" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A137" s="4" t="s">
         <v>149</v>
       </c>
@@ -6071,7 +6071,7 @@
       <c r="I137" s="6"/>
       <c r="J137" s="7"/>
     </row>
-    <row r="138" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A138" s="4" t="s">
         <v>150</v>
       </c>
@@ -6099,7 +6099,7 @@
       <c r="I138" s="6"/>
       <c r="J138" s="7"/>
     </row>
-    <row r="139" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A139" s="4" t="s">
         <v>151</v>
       </c>
@@ -6125,7 +6125,7 @@
       <c r="I139" s="6"/>
       <c r="J139" s="7"/>
     </row>
-    <row r="140" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A140" s="4" t="s">
         <v>152</v>
       </c>
@@ -6153,7 +6153,7 @@
       <c r="I140" s="6"/>
       <c r="J140" s="7"/>
     </row>
-    <row r="141" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A141" s="4" t="s">
         <v>153</v>
       </c>
@@ -6181,7 +6181,7 @@
       <c r="I141" s="6"/>
       <c r="J141" s="7"/>
     </row>
-    <row r="142" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A142" s="4" t="s">
         <v>154</v>
       </c>
@@ -6209,7 +6209,7 @@
       <c r="I142" s="6"/>
       <c r="J142" s="7"/>
     </row>
-    <row r="143" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A143" s="4" t="s">
         <v>155</v>
       </c>
@@ -6235,7 +6235,7 @@
       <c r="I143" s="6"/>
       <c r="J143" s="7"/>
     </row>
-    <row r="144" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A144" s="4" t="s">
         <v>156</v>
       </c>
@@ -6261,7 +6261,7 @@
       <c r="I144" s="6"/>
       <c r="J144" s="7"/>
     </row>
-    <row r="145" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A145" s="4" t="s">
         <v>157</v>
       </c>
@@ -6289,7 +6289,7 @@
       <c r="I145" s="6"/>
       <c r="J145" s="7"/>
     </row>
-    <row r="146" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A146" s="4" t="s">
         <v>158</v>
       </c>
@@ -6317,7 +6317,7 @@
       <c r="I146" s="6"/>
       <c r="J146" s="7"/>
     </row>
-    <row r="147" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A147" s="4" t="s">
         <v>159</v>
       </c>
@@ -6345,7 +6345,7 @@
       <c r="I147" s="6"/>
       <c r="J147" s="7"/>
     </row>
-    <row r="148" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A148" s="4" t="s">
         <v>160</v>
       </c>
@@ -6373,7 +6373,7 @@
       <c r="I148" s="6"/>
       <c r="J148" s="7"/>
     </row>
-    <row r="149" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A149" s="4" t="s">
         <v>161</v>
       </c>
@@ -6401,7 +6401,7 @@
       <c r="I149" s="6"/>
       <c r="J149" s="7"/>
     </row>
-    <row r="150" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A150" s="4" t="s">
         <v>162</v>
       </c>
@@ -6429,7 +6429,7 @@
       <c r="I150" s="6"/>
       <c r="J150" s="7"/>
     </row>
-    <row r="151" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A151" s="4" t="s">
         <v>163</v>
       </c>
@@ -6455,7 +6455,7 @@
       <c r="I151" s="6"/>
       <c r="J151" s="7"/>
     </row>
-    <row r="152" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A152" s="4" t="s">
         <v>164</v>
       </c>
@@ -6483,7 +6483,7 @@
       <c r="I152" s="6"/>
       <c r="J152" s="7"/>
     </row>
-    <row r="153" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A153" s="4" t="s">
         <v>165</v>
       </c>
@@ -6511,7 +6511,7 @@
       <c r="I153" s="6"/>
       <c r="J153" s="7"/>
     </row>
-    <row r="154" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A154" s="4" t="s">
         <v>166</v>
       </c>
@@ -6539,7 +6539,7 @@
       <c r="I154" s="6"/>
       <c r="J154" s="7"/>
     </row>
-    <row r="155" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A155" s="4" t="s">
         <v>167</v>
       </c>
@@ -6567,7 +6567,7 @@
       <c r="I155" s="6"/>
       <c r="J155" s="7"/>
     </row>
-    <row r="156" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A156" s="4" t="s">
         <v>168</v>
       </c>
@@ -6595,7 +6595,7 @@
       <c r="I156" s="6"/>
       <c r="J156" s="7"/>
     </row>
-    <row r="157" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A157" s="4" t="s">
         <v>169</v>
       </c>
@@ -6623,7 +6623,7 @@
       <c r="I157" s="6"/>
       <c r="J157" s="7"/>
     </row>
-    <row r="158" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A158" s="4" t="s">
         <v>170</v>
       </c>
@@ -6651,7 +6651,7 @@
       <c r="I158" s="6"/>
       <c r="J158" s="7"/>
     </row>
-    <row r="159" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A159" s="4" t="s">
         <v>171</v>
       </c>
@@ -6679,7 +6679,7 @@
       <c r="I159" s="6"/>
       <c r="J159" s="7"/>
     </row>
-    <row r="160" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A160" s="4" t="s">
         <v>172</v>
       </c>
@@ -6707,7 +6707,7 @@
       <c r="I160" s="6"/>
       <c r="J160" s="7"/>
     </row>
-    <row r="161" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A161" s="4" t="s">
         <v>173</v>
       </c>
@@ -6735,7 +6735,7 @@
       <c r="I161" s="6"/>
       <c r="J161" s="7"/>
     </row>
-    <row r="162" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A162" s="4" t="s">
         <v>174</v>
       </c>
@@ -6763,7 +6763,7 @@
       <c r="I162" s="6"/>
       <c r="J162" s="7"/>
     </row>
-    <row r="163" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A163" s="4" t="s">
         <v>175</v>
       </c>
@@ -6791,7 +6791,7 @@
       <c r="I163" s="6"/>
       <c r="J163" s="7"/>
     </row>
-    <row r="164" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A164" s="4" t="s">
         <v>176</v>
       </c>
@@ -6819,7 +6819,7 @@
       <c r="I164" s="6"/>
       <c r="J164" s="7"/>
     </row>
-    <row r="165" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A165" s="4" t="s">
         <v>177</v>
       </c>
@@ -6845,7 +6845,7 @@
       <c r="I165" s="6"/>
       <c r="J165" s="7"/>
     </row>
-    <row r="166" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A166" s="4" t="s">
         <v>178</v>
       </c>
@@ -6873,7 +6873,7 @@
       <c r="I166" s="6"/>
       <c r="J166" s="7"/>
     </row>
-    <row r="167" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A167" s="4" t="s">
         <v>179</v>
       </c>
@@ -6901,7 +6901,7 @@
       <c r="I167" s="6"/>
       <c r="J167" s="7"/>
     </row>
-    <row r="168" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A168" s="4" t="s">
         <v>180</v>
       </c>
@@ -6929,7 +6929,7 @@
       <c r="I168" s="6"/>
       <c r="J168" s="7"/>
     </row>
-    <row r="169" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A169" s="4" t="s">
         <v>181</v>
       </c>
@@ -6957,7 +6957,7 @@
       <c r="I169" s="6"/>
       <c r="J169" s="7"/>
     </row>
-    <row r="170" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A170" s="4" t="s">
         <v>182</v>
       </c>
@@ -6985,7 +6985,7 @@
       <c r="I170" s="6"/>
       <c r="J170" s="7"/>
     </row>
-    <row r="171" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A171" s="4" t="s">
         <v>183</v>
       </c>
@@ -7013,7 +7013,7 @@
       <c r="I171" s="6"/>
       <c r="J171" s="7"/>
     </row>
-    <row r="172" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A172" s="4" t="s">
         <v>184</v>
       </c>
@@ -7041,7 +7041,7 @@
       <c r="I172" s="6"/>
       <c r="J172" s="7"/>
     </row>
-    <row r="173" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A173" s="4" t="s">
         <v>185</v>
       </c>
@@ -7069,7 +7069,7 @@
       <c r="I173" s="6"/>
       <c r="J173" s="7"/>
     </row>
-    <row r="174" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A174" s="4" t="s">
         <v>186</v>
       </c>
@@ -7097,7 +7097,7 @@
       <c r="I174" s="6"/>
       <c r="J174" s="7"/>
     </row>
-    <row r="175" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A175" s="4" t="s">
         <v>187</v>
       </c>
@@ -7125,7 +7125,7 @@
       <c r="I175" s="6"/>
       <c r="J175" s="7"/>
     </row>
-    <row r="176" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A176" s="4" t="s">
         <v>188</v>
       </c>
@@ -7153,7 +7153,7 @@
       <c r="I176" s="6"/>
       <c r="J176" s="7"/>
     </row>
-    <row r="177" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A177" s="4" t="s">
         <v>189</v>
       </c>
@@ -7181,7 +7181,7 @@
       <c r="I177" s="6"/>
       <c r="J177" s="7"/>
     </row>
-    <row r="178" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A178" s="4" t="s">
         <v>190</v>
       </c>
@@ -7209,7 +7209,7 @@
       <c r="I178" s="6"/>
       <c r="J178" s="7"/>
     </row>
-    <row r="179" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A179" s="4" t="s">
         <v>191</v>
       </c>
@@ -7237,7 +7237,7 @@
       <c r="I179" s="6"/>
       <c r="J179" s="7"/>
     </row>
-    <row r="180" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A180" s="4" t="s">
         <v>192</v>
       </c>
@@ -7265,7 +7265,7 @@
       <c r="I180" s="6"/>
       <c r="J180" s="7"/>
     </row>
-    <row r="181" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A181" s="4" t="s">
         <v>193</v>
       </c>
@@ -7293,7 +7293,7 @@
       <c r="I181" s="6"/>
       <c r="J181" s="7"/>
     </row>
-    <row r="182" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A182" s="4" t="s">
         <v>194</v>
       </c>
@@ -7321,7 +7321,7 @@
       <c r="I182" s="6"/>
       <c r="J182" s="7"/>
     </row>
-    <row r="183" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A183" s="4" t="s">
         <v>195</v>
       </c>
@@ -7349,7 +7349,7 @@
       <c r="I183" s="6"/>
       <c r="J183" s="7"/>
     </row>
-    <row r="184" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A184" s="4" t="s">
         <v>196</v>
       </c>
@@ -7377,7 +7377,7 @@
       <c r="I184" s="6"/>
       <c r="J184" s="7"/>
     </row>
-    <row r="185" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A185" s="4" t="s">
         <v>197</v>
       </c>
@@ -7405,7 +7405,7 @@
       <c r="I185" s="6"/>
       <c r="J185" s="7"/>
     </row>
-    <row r="186" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A186" s="4" t="s">
         <v>198</v>
       </c>
@@ -7433,7 +7433,7 @@
       <c r="I186" s="6"/>
       <c r="J186" s="7"/>
     </row>
-    <row r="187" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A187" s="4" t="s">
         <v>199</v>
       </c>
@@ -7461,7 +7461,7 @@
       <c r="I187" s="6"/>
       <c r="J187" s="7"/>
     </row>
-    <row r="188" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A188" s="4" t="s">
         <v>200</v>
       </c>
@@ -7489,7 +7489,7 @@
       <c r="I188" s="6"/>
       <c r="J188" s="7"/>
     </row>
-    <row r="189" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A189" s="4" t="s">
         <v>201</v>
       </c>
@@ -7517,7 +7517,7 @@
       <c r="I189" s="6"/>
       <c r="J189" s="7"/>
     </row>
-    <row r="190" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A190" s="4" t="s">
         <v>202</v>
       </c>
@@ -7545,7 +7545,7 @@
       <c r="I190" s="6"/>
       <c r="J190" s="7"/>
     </row>
-    <row r="191" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A191" s="4" t="s">
         <v>203</v>
       </c>
@@ -7573,7 +7573,7 @@
       <c r="I191" s="6"/>
       <c r="J191" s="7"/>
     </row>
-    <row r="192" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A192" s="4" t="s">
         <v>204</v>
       </c>
@@ -7601,7 +7601,7 @@
       <c r="I192" s="6"/>
       <c r="J192" s="7"/>
     </row>
-    <row r="193" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A193" s="4" t="s">
         <v>205</v>
       </c>
@@ -7629,7 +7629,7 @@
       <c r="I193" s="6"/>
       <c r="J193" s="7"/>
     </row>
-    <row r="194" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A194" s="4" t="s">
         <v>206</v>
       </c>
@@ -7657,7 +7657,7 @@
       <c r="I194" s="6"/>
       <c r="J194" s="7"/>
     </row>
-    <row r="195" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A195" s="4" t="s">
         <v>207</v>
       </c>
@@ -7685,7 +7685,7 @@
       <c r="I195" s="6"/>
       <c r="J195" s="7"/>
     </row>
-    <row r="196" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A196" s="4" t="s">
         <v>208</v>
       </c>
@@ -7713,7 +7713,7 @@
       <c r="I196" s="6"/>
       <c r="J196" s="7"/>
     </row>
-    <row r="197" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A197" s="4" t="s">
         <v>209</v>
       </c>
@@ -7741,7 +7741,7 @@
       <c r="I197" s="6"/>
       <c r="J197" s="7"/>
     </row>
-    <row r="198" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A198" s="4" t="s">
         <v>210</v>
       </c>
@@ -7769,7 +7769,7 @@
       <c r="I198" s="6"/>
       <c r="J198" s="7"/>
     </row>
-    <row r="199" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A199" s="4" t="s">
         <v>211</v>
       </c>
@@ -7797,7 +7797,7 @@
       <c r="I199" s="6"/>
       <c r="J199" s="7"/>
     </row>
-    <row r="200" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A200" s="4" t="s">
         <v>212</v>
       </c>
@@ -7825,7 +7825,7 @@
       <c r="I200" s="6"/>
       <c r="J200" s="7"/>
     </row>
-    <row r="201" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A201" s="4" t="s">
         <v>213</v>
       </c>
@@ -7851,7 +7851,7 @@
       <c r="I201" s="6"/>
       <c r="J201" s="7"/>
     </row>
-    <row r="202" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A202" s="4" t="s">
         <v>214</v>
       </c>
@@ -7879,7 +7879,7 @@
       <c r="I202" s="6"/>
       <c r="J202" s="7"/>
     </row>
-    <row r="203" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A203" s="4" t="s">
         <v>215</v>
       </c>
@@ -7907,7 +7907,7 @@
       <c r="I203" s="6"/>
       <c r="J203" s="7"/>
     </row>
-    <row r="204" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A204" s="4" t="s">
         <v>216</v>
       </c>
@@ -7935,7 +7935,7 @@
       <c r="I204" s="6"/>
       <c r="J204" s="7"/>
     </row>
-    <row r="205" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A205" s="4" t="s">
         <v>217</v>
       </c>
@@ -7963,7 +7963,7 @@
       <c r="I205" s="6"/>
       <c r="J205" s="7"/>
     </row>
-    <row r="206" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A206" s="4" t="s">
         <v>218</v>
       </c>
@@ -7991,7 +7991,7 @@
       <c r="I206" s="6"/>
       <c r="J206" s="7"/>
     </row>
-    <row r="207" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A207" s="4" t="s">
         <v>219</v>
       </c>
@@ -8019,7 +8019,7 @@
       <c r="I207" s="6"/>
       <c r="J207" s="7"/>
     </row>
-    <row r="208" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A208" s="4" t="s">
         <v>220</v>
       </c>
@@ -8047,7 +8047,7 @@
       <c r="I208" s="6"/>
       <c r="J208" s="7"/>
     </row>
-    <row r="209" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A209" s="4" t="s">
         <v>221</v>
       </c>
@@ -8075,7 +8075,7 @@
       <c r="I209" s="6"/>
       <c r="J209" s="7"/>
     </row>
-    <row r="210" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A210" s="4" t="s">
         <v>222</v>
       </c>
@@ -8103,7 +8103,7 @@
       <c r="I210" s="6"/>
       <c r="J210" s="7"/>
     </row>
-    <row r="211" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A211" s="4" t="s">
         <v>223</v>
       </c>
@@ -8131,7 +8131,7 @@
       <c r="I211" s="6"/>
       <c r="J211" s="7"/>
     </row>
-    <row r="212" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A212" s="4" t="s">
         <v>224</v>
       </c>
@@ -8159,7 +8159,7 @@
       <c r="I212" s="6"/>
       <c r="J212" s="7"/>
     </row>
-    <row r="213" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A213" s="4" t="s">
         <v>225</v>
       </c>
@@ -8187,7 +8187,7 @@
       <c r="I213" s="6"/>
       <c r="J213" s="7"/>
     </row>
-    <row r="214" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A214" s="4" t="s">
         <v>226</v>
       </c>
@@ -8213,7 +8213,7 @@
       <c r="I214" s="6"/>
       <c r="J214" s="7"/>
     </row>
-    <row r="215" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="215" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A215" s="4" t="s">
         <v>227</v>
       </c>
@@ -8241,7 +8241,7 @@
       <c r="I215" s="6"/>
       <c r="J215" s="7"/>
     </row>
-    <row r="216" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A216" s="9" t="s">
         <v>228</v>
       </c>
@@ -8265,7 +8265,7 @@
       <c r="I216" s="11"/>
       <c r="J216" s="12"/>
     </row>
-    <row r="217" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A217" s="4" t="s">
         <v>230</v>
       </c>
@@ -8291,7 +8291,7 @@
       <c r="I217" s="6"/>
       <c r="J217" s="7"/>
     </row>
-    <row r="218" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A218" s="4" t="s">
         <v>231</v>
       </c>
@@ -8313,7 +8313,7 @@
       <c r="I218" s="6"/>
       <c r="J218" s="7"/>
     </row>
-    <row r="219" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A219" s="4" t="s">
         <v>232</v>
       </c>
@@ -8335,7 +8335,7 @@
       <c r="I219" s="6"/>
       <c r="J219" s="7"/>
     </row>
-    <row r="220" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A220" s="4" t="s">
         <v>233</v>
       </c>
@@ -8361,7 +8361,7 @@
       <c r="I220" s="6"/>
       <c r="J220" s="7"/>
     </row>
-    <row r="221" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A221" s="4" t="s">
         <v>234</v>
       </c>
@@ -8387,7 +8387,7 @@
       <c r="I221" s="6"/>
       <c r="J221" s="7"/>
     </row>
-    <row r="222" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A222" s="4" t="s">
         <v>235</v>
       </c>
@@ -8409,7 +8409,7 @@
       <c r="I222" s="6"/>
       <c r="J222" s="7"/>
     </row>
-    <row r="223" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A223" s="4" t="s">
         <v>236</v>
       </c>
@@ -8435,7 +8435,7 @@
       <c r="I223" s="6"/>
       <c r="J223" s="7"/>
     </row>
-    <row r="224" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A224" s="4" t="s">
         <v>237</v>
       </c>
@@ -8461,7 +8461,7 @@
       <c r="I224" s="6"/>
       <c r="J224" s="7"/>
     </row>
-    <row r="225" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A225" s="4" t="s">
         <v>238</v>
       </c>
@@ -8483,7 +8483,7 @@
       <c r="I225" s="6"/>
       <c r="J225" s="7"/>
     </row>
-    <row r="226" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A226" s="4" t="s">
         <v>239</v>
       </c>
@@ -8505,7 +8505,7 @@
       <c r="I226" s="6"/>
       <c r="J226" s="7"/>
     </row>
-    <row r="227" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A227" s="4" t="s">
         <v>240</v>
       </c>
@@ -8527,7 +8527,7 @@
       <c r="I227" s="6"/>
       <c r="J227" s="7"/>
     </row>
-    <row r="228" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A228" s="4" t="s">
         <v>241</v>
       </c>
@@ -8549,7 +8549,7 @@
       <c r="I228" s="6"/>
       <c r="J228" s="7"/>
     </row>
-    <row r="229" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A229" s="4" t="s">
         <v>242</v>
       </c>
@@ -8571,7 +8571,7 @@
       <c r="I229" s="6"/>
       <c r="J229" s="7"/>
     </row>
-    <row r="230" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A230" s="4" t="s">
         <v>243</v>
       </c>
@@ -8593,7 +8593,7 @@
       <c r="I230" s="6"/>
       <c r="J230" s="7"/>
     </row>
-    <row r="231" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="231" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A231" s="4" t="s">
         <v>244</v>
       </c>
@@ -8619,7 +8619,7 @@
       <c r="I231" s="6"/>
       <c r="J231" s="7"/>
     </row>
-    <row r="232" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="232" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A232" s="4" t="s">
         <v>245</v>
       </c>
@@ -8645,7 +8645,7 @@
       <c r="I232" s="6"/>
       <c r="J232" s="7"/>
     </row>
-    <row r="233" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="233" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A233" s="4" t="s">
         <v>246</v>
       </c>
@@ -8671,7 +8671,7 @@
       <c r="I233" s="6"/>
       <c r="J233" s="7"/>
     </row>
-    <row r="234" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="234" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A234" s="4" t="s">
         <v>247</v>
       </c>
@@ -8693,7 +8693,7 @@
       <c r="I234" s="6"/>
       <c r="J234" s="7"/>
     </row>
-    <row r="235" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="235" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A235" s="4" t="s">
         <v>248</v>
       </c>
@@ -8715,7 +8715,7 @@
       <c r="I235" s="6"/>
       <c r="J235" s="7"/>
     </row>
-    <row r="236" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="236" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A236" s="4" t="s">
         <v>249</v>
       </c>
@@ -8737,7 +8737,7 @@
       <c r="I236" s="6"/>
       <c r="J236" s="7"/>
     </row>
-    <row r="237" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="237" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A237" s="4" t="s">
         <v>250</v>
       </c>
@@ -8759,7 +8759,7 @@
       <c r="I237" s="6"/>
       <c r="J237" s="7"/>
     </row>
-    <row r="238" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="238" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A238" s="4" t="s">
         <v>251</v>
       </c>
@@ -8781,7 +8781,7 @@
       <c r="I238" s="6"/>
       <c r="J238" s="7"/>
     </row>
-    <row r="239" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="239" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A239" s="4" t="s">
         <v>252</v>
       </c>
@@ -8803,7 +8803,7 @@
       <c r="I239" s="6"/>
       <c r="J239" s="7"/>
     </row>
-    <row r="240" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="240" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A240" s="4" t="s">
         <v>253</v>
       </c>
@@ -8825,7 +8825,7 @@
       <c r="I240" s="6"/>
       <c r="J240" s="7"/>
     </row>
-    <row r="241" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="241" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A241" s="4" t="s">
         <v>254</v>
       </c>
@@ -8847,7 +8847,7 @@
       <c r="I241" s="6"/>
       <c r="J241" s="7"/>
     </row>
-    <row r="242" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="242" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A242" s="4" t="s">
         <v>255</v>
       </c>
@@ -8869,7 +8869,7 @@
       <c r="I242" s="6"/>
       <c r="J242" s="7"/>
     </row>
-    <row r="243" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="243" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A243" s="4" t="s">
         <v>256</v>
       </c>
@@ -8895,7 +8895,7 @@
       <c r="I243" s="6"/>
       <c r="J243" s="7"/>
     </row>
-    <row r="244" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="244" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A244" s="13" t="s">
         <v>257</v>
       </c>
@@ -8921,7 +8921,7 @@
       <c r="I244" s="15"/>
       <c r="J244" s="16"/>
     </row>
-    <row r="245" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="245" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A245" s="4" t="s">
         <v>258</v>
       </c>
@@ -8947,7 +8947,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="246" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="246" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A246" s="4" t="s">
         <v>260</v>
       </c>
@@ -8973,7 +8973,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="247" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="247" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A247" s="4" t="s">
         <v>261</v>
       </c>
@@ -8999,7 +8999,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="248" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="248" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A248" s="4" t="s">
         <v>262</v>
       </c>
@@ -9025,7 +9025,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="249" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="249" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A249" s="4" t="s">
         <v>263</v>
       </c>
@@ -9051,7 +9051,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="250" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="250" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A250" s="4" t="s">
         <v>264</v>
       </c>
@@ -9077,7 +9077,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="251" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="251" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A251" s="4" t="s">
         <v>265</v>
       </c>
@@ -9103,7 +9103,7 @@
         <v>558</v>
       </c>
     </row>
-    <row r="252" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="252" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A252" s="4" t="s">
         <v>266</v>
       </c>
@@ -9129,7 +9129,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="253" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="253" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A253" s="4" t="s">
         <v>267</v>
       </c>
@@ -9155,7 +9155,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="254" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="254" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A254" s="4" t="s">
         <v>268</v>
       </c>
@@ -9181,7 +9181,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="255" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="255" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A255" s="4" t="s">
         <v>269</v>
       </c>
@@ -9207,7 +9207,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="256" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="256" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A256" s="4" t="s">
         <v>270</v>
       </c>
@@ -9233,7 +9233,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="257" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="257" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A257" s="4" t="s">
         <v>271</v>
       </c>
@@ -9259,7 +9259,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="258" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="258" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A258" s="4" t="s">
         <v>272</v>
       </c>
@@ -9285,7 +9285,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="259" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="259" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A259" s="4" t="s">
         <v>273</v>
       </c>
@@ -9311,7 +9311,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="260" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="260" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A260" s="4" t="s">
         <v>274</v>
       </c>
@@ -9337,7 +9337,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="261" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="261" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A261" s="4" t="s">
         <v>275</v>
       </c>
@@ -9363,7 +9363,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="262" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="262" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A262" s="4" t="s">
         <v>276</v>
       </c>
@@ -9389,7 +9389,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="263" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="263" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A263" s="4" t="s">
         <v>277</v>
       </c>
@@ -9415,7 +9415,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="264" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="264" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A264" s="4" t="s">
         <v>278</v>
       </c>
@@ -9437,7 +9437,7 @@
       <c r="I264" s="6"/>
       <c r="J264" s="7"/>
     </row>
-    <row r="265" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="265" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A265" s="4" t="s">
         <v>279</v>
       </c>
@@ -9459,7 +9459,7 @@
       <c r="I265" s="6"/>
       <c r="J265" s="7"/>
     </row>
-    <row r="266" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="266" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A266" s="4" t="s">
         <v>280</v>
       </c>
@@ -9481,7 +9481,7 @@
       <c r="I266" s="6"/>
       <c r="J266" s="7"/>
     </row>
-    <row r="267" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="267" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A267" s="4" t="s">
         <v>281</v>
       </c>
@@ -9503,7 +9503,7 @@
       <c r="I267" s="6"/>
       <c r="J267" s="7"/>
     </row>
-    <row r="268" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="268" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A268" s="4" t="s">
         <v>282</v>
       </c>
@@ -9525,7 +9525,7 @@
       <c r="I268" s="6"/>
       <c r="J268" s="7"/>
     </row>
-    <row r="269" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="269" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A269" s="4" t="s">
         <v>283</v>
       </c>
@@ -9547,7 +9547,7 @@
       <c r="I269" s="6"/>
       <c r="J269" s="7"/>
     </row>
-    <row r="270" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="270" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A270" s="4" t="s">
         <v>284</v>
       </c>
@@ -9569,7 +9569,7 @@
       <c r="I270" s="6"/>
       <c r="J270" s="7"/>
     </row>
-    <row r="271" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="271" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A271" s="4" t="s">
         <v>285</v>
       </c>
@@ -9591,7 +9591,7 @@
       <c r="I271" s="6"/>
       <c r="J271" s="7"/>
     </row>
-    <row r="272" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="272" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A272" s="4" t="s">
         <v>286</v>
       </c>
@@ -9613,7 +9613,7 @@
       <c r="I272" s="6"/>
       <c r="J272" s="7"/>
     </row>
-    <row r="273" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="273" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A273" s="4" t="s">
         <v>287</v>
       </c>
@@ -9635,7 +9635,7 @@
       <c r="I273" s="6"/>
       <c r="J273" s="7"/>
     </row>
-    <row r="274" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="274" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A274" s="4" t="s">
         <v>288</v>
       </c>
@@ -9657,7 +9657,7 @@
       <c r="I274" s="6"/>
       <c r="J274" s="7"/>
     </row>
-    <row r="275" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="275" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A275" s="4" t="s">
         <v>289</v>
       </c>
@@ -9679,7 +9679,7 @@
       <c r="I275" s="6"/>
       <c r="J275" s="7"/>
     </row>
-    <row r="276" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="276" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A276" s="4" t="s">
         <v>290</v>
       </c>
@@ -9701,7 +9701,7 @@
       <c r="I276" s="6"/>
       <c r="J276" s="7"/>
     </row>
-    <row r="277" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="277" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A277" s="4" t="s">
         <v>291</v>
       </c>
@@ -9723,7 +9723,7 @@
       <c r="I277" s="6"/>
       <c r="J277" s="7"/>
     </row>
-    <row r="278" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="278" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A278" s="4" t="s">
         <v>292</v>
       </c>
@@ -9745,7 +9745,7 @@
       <c r="I278" s="6"/>
       <c r="J278" s="7"/>
     </row>
-    <row r="279" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="279" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A279" s="4" t="s">
         <v>293</v>
       </c>
@@ -9767,7 +9767,7 @@
       <c r="I279" s="6"/>
       <c r="J279" s="7"/>
     </row>
-    <row r="280" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="280" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A280" s="4" t="s">
         <v>294</v>
       </c>
@@ -9789,7 +9789,7 @@
       <c r="I280" s="6"/>
       <c r="J280" s="7"/>
     </row>
-    <row r="281" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="281" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A281" s="4" t="s">
         <v>295</v>
       </c>
@@ -9811,7 +9811,7 @@
       <c r="I281" s="6"/>
       <c r="J281" s="7"/>
     </row>
-    <row r="282" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="282" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A282" s="4" t="s">
         <v>296</v>
       </c>
@@ -9833,7 +9833,7 @@
       <c r="I282" s="6"/>
       <c r="J282" s="7"/>
     </row>
-    <row r="283" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="283" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A283" s="4" t="s">
         <v>297</v>
       </c>
@@ -9855,7 +9855,7 @@
       <c r="I283" s="6"/>
       <c r="J283" s="7"/>
     </row>
-    <row r="284" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="284" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A284" s="4" t="s">
         <v>298</v>
       </c>
@@ -9877,7 +9877,7 @@
       <c r="I284" s="6"/>
       <c r="J284" s="7"/>
     </row>
-    <row r="285" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="285" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A285" s="4" t="s">
         <v>299</v>
       </c>
@@ -9899,7 +9899,7 @@
       <c r="I285" s="6"/>
       <c r="J285" s="7"/>
     </row>
-    <row r="286" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="286" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A286" s="4" t="s">
         <v>300</v>
       </c>
@@ -9921,7 +9921,7 @@
       <c r="I286" s="6"/>
       <c r="J286" s="7"/>
     </row>
-    <row r="287" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="287" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A287" s="4" t="s">
         <v>301</v>
       </c>
@@ -9943,7 +9943,7 @@
       <c r="I287" s="6"/>
       <c r="J287" s="7"/>
     </row>
-    <row r="288" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="288" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A288" s="4" t="s">
         <v>302</v>
       </c>
@@ -9965,7 +9965,7 @@
       <c r="I288" s="6"/>
       <c r="J288" s="7"/>
     </row>
-    <row r="289" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="289" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A289" s="4" t="s">
         <v>303</v>
       </c>
@@ -9987,7 +9987,7 @@
       <c r="I289" s="6"/>
       <c r="J289" s="7"/>
     </row>
-    <row r="290" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="290" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A290" s="4" t="s">
         <v>304</v>
       </c>
@@ -10009,7 +10009,7 @@
       <c r="I290" s="6"/>
       <c r="J290" s="7"/>
     </row>
-    <row r="291" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="291" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A291" s="4" t="s">
         <v>305</v>
       </c>
@@ -10031,7 +10031,7 @@
       <c r="I291" s="6"/>
       <c r="J291" s="7"/>
     </row>
-    <row r="292" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="292" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A292" s="4" t="s">
         <v>306</v>
       </c>
@@ -10053,7 +10053,7 @@
       <c r="I292" s="6"/>
       <c r="J292" s="7"/>
     </row>
-    <row r="293" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="293" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A293" s="4" t="s">
         <v>307</v>
       </c>
@@ -10075,7 +10075,7 @@
       <c r="I293" s="6"/>
       <c r="J293" s="7"/>
     </row>
-    <row r="294" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="294" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A294" s="4" t="s">
         <v>308</v>
       </c>
@@ -10097,7 +10097,7 @@
       <c r="I294" s="6"/>
       <c r="J294" s="7"/>
     </row>
-    <row r="295" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="295" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A295" s="4" t="s">
         <v>309</v>
       </c>
@@ -10119,7 +10119,7 @@
       <c r="I295" s="6"/>
       <c r="J295" s="7"/>
     </row>
-    <row r="296" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="296" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A296" s="4" t="s">
         <v>310</v>
       </c>
@@ -10141,7 +10141,7 @@
       <c r="I296" s="6"/>
       <c r="J296" s="7"/>
     </row>
-    <row r="297" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="297" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A297" s="4" t="s">
         <v>311</v>
       </c>
@@ -10163,7 +10163,7 @@
       <c r="I297" s="6"/>
       <c r="J297" s="7"/>
     </row>
-    <row r="298" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="298" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A298" s="4" t="s">
         <v>312</v>
       </c>
@@ -10185,7 +10185,7 @@
       <c r="I298" s="6"/>
       <c r="J298" s="7"/>
     </row>
-    <row r="299" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="299" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A299" s="4" t="s">
         <v>313</v>
       </c>
@@ -10207,7 +10207,7 @@
       <c r="I299" s="6"/>
       <c r="J299" s="7"/>
     </row>
-    <row r="300" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="300" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A300" s="4" t="s">
         <v>314</v>
       </c>
@@ -10229,7 +10229,7 @@
       <c r="I300" s="6"/>
       <c r="J300" s="7"/>
     </row>
-    <row r="301" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="301" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A301" s="4" t="s">
         <v>315</v>
       </c>
@@ -10251,7 +10251,7 @@
       <c r="I301" s="6"/>
       <c r="J301" s="7"/>
     </row>
-    <row r="302" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="302" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A302" s="4" t="s">
         <v>316</v>
       </c>
@@ -10273,7 +10273,7 @@
       <c r="I302" s="6"/>
       <c r="J302" s="7"/>
     </row>
-    <row r="303" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="303" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A303" s="4" t="s">
         <v>317</v>
       </c>
@@ -10295,7 +10295,7 @@
       <c r="I303" s="6"/>
       <c r="J303" s="7"/>
     </row>
-    <row r="304" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="304" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A304" s="4" t="s">
         <v>318</v>
       </c>
@@ -10317,7 +10317,7 @@
       <c r="I304" s="6"/>
       <c r="J304" s="7"/>
     </row>
-    <row r="305" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="305" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A305" s="4" t="s">
         <v>319</v>
       </c>
@@ -10339,7 +10339,7 @@
       <c r="I305" s="6"/>
       <c r="J305" s="7"/>
     </row>
-    <row r="306" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="306" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A306" s="4" t="s">
         <v>320</v>
       </c>
@@ -10361,7 +10361,7 @@
       <c r="I306" s="6"/>
       <c r="J306" s="7"/>
     </row>
-    <row r="307" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="307" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A307" s="4" t="s">
         <v>321</v>
       </c>
@@ -10383,7 +10383,7 @@
       <c r="I307" s="6"/>
       <c r="J307" s="7"/>
     </row>
-    <row r="308" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="308" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A308" s="4" t="s">
         <v>322</v>
       </c>
@@ -10405,7 +10405,7 @@
       <c r="I308" s="6"/>
       <c r="J308" s="7"/>
     </row>
-    <row r="309" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="309" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A309" s="4" t="s">
         <v>323</v>
       </c>
@@ -10427,7 +10427,7 @@
       <c r="I309" s="6"/>
       <c r="J309" s="7"/>
     </row>
-    <row r="310" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="310" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A310" s="4" t="s">
         <v>324</v>
       </c>
@@ -10449,7 +10449,7 @@
       <c r="I310" s="6"/>
       <c r="J310" s="7"/>
     </row>
-    <row r="311" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="311" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A311" s="4" t="s">
         <v>325</v>
       </c>
@@ -10471,7 +10471,7 @@
       <c r="I311" s="6"/>
       <c r="J311" s="7"/>
     </row>
-    <row r="312" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="312" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A312" s="4" t="s">
         <v>326</v>
       </c>
@@ -10493,7 +10493,7 @@
       <c r="I312" s="6"/>
       <c r="J312" s="7"/>
     </row>
-    <row r="313" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="313" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A313" s="4" t="s">
         <v>327</v>
       </c>
@@ -10515,7 +10515,7 @@
       <c r="I313" s="6"/>
       <c r="J313" s="7"/>
     </row>
-    <row r="314" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="314" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A314" s="4" t="s">
         <v>328</v>
       </c>
@@ -10537,7 +10537,7 @@
       <c r="I314" s="6"/>
       <c r="J314" s="7"/>
     </row>
-    <row r="315" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="315" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A315" s="4" t="s">
         <v>329</v>
       </c>
@@ -10559,7 +10559,7 @@
       <c r="I315" s="6"/>
       <c r="J315" s="7"/>
     </row>
-    <row r="316" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="316" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A316" s="4" t="s">
         <v>330</v>
       </c>
@@ -10581,7 +10581,7 @@
       <c r="I316" s="6"/>
       <c r="J316" s="7"/>
     </row>
-    <row r="317" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="317" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A317" s="4" t="s">
         <v>331</v>
       </c>
@@ -10603,7 +10603,7 @@
       <c r="I317" s="6"/>
       <c r="J317" s="7"/>
     </row>
-    <row r="318" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="318" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A318" s="4" t="s">
         <v>332</v>
       </c>
@@ -10625,7 +10625,7 @@
       <c r="I318" s="6"/>
       <c r="J318" s="7"/>
     </row>
-    <row r="319" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="319" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A319" s="4" t="s">
         <v>333</v>
       </c>
@@ -10647,7 +10647,7 @@
       <c r="I319" s="6"/>
       <c r="J319" s="7"/>
     </row>
-    <row r="320" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="320" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A320" s="4" t="s">
         <v>334</v>
       </c>
@@ -10669,7 +10669,7 @@
       <c r="I320" s="6"/>
       <c r="J320" s="7"/>
     </row>
-    <row r="321" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="321" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A321" s="4" t="s">
         <v>335</v>
       </c>
@@ -10691,7 +10691,7 @@
       <c r="I321" s="6"/>
       <c r="J321" s="7"/>
     </row>
-    <row r="322" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="322" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A322" s="4" t="s">
         <v>336</v>
       </c>
@@ -10713,7 +10713,7 @@
       <c r="I322" s="6"/>
       <c r="J322" s="7"/>
     </row>
-    <row r="323" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="323" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A323" s="4" t="s">
         <v>337</v>
       </c>
@@ -10735,7 +10735,7 @@
       <c r="I323" s="6"/>
       <c r="J323" s="7"/>
     </row>
-    <row r="324" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="324" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A324" s="4" t="s">
         <v>338</v>
       </c>
@@ -10757,7 +10757,7 @@
       <c r="I324" s="6"/>
       <c r="J324" s="7"/>
     </row>
-    <row r="325" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="325" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A325" s="4" t="s">
         <v>339</v>
       </c>
@@ -10779,7 +10779,7 @@
       <c r="I325" s="6"/>
       <c r="J325" s="7"/>
     </row>
-    <row r="326" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="326" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A326" s="4" t="s">
         <v>340</v>
       </c>
@@ -10801,7 +10801,7 @@
       <c r="I326" s="6"/>
       <c r="J326" s="7"/>
     </row>
-    <row r="327" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="327" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A327" s="4" t="s">
         <v>341</v>
       </c>
@@ -10823,7 +10823,7 @@
       <c r="I327" s="6"/>
       <c r="J327" s="7"/>
     </row>
-    <row r="328" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="328" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A328" s="4" t="s">
         <v>342</v>
       </c>
@@ -10845,7 +10845,7 @@
       <c r="I328" s="6"/>
       <c r="J328" s="7"/>
     </row>
-    <row r="329" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="329" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A329" s="4" t="s">
         <v>343</v>
       </c>
@@ -10867,7 +10867,7 @@
       <c r="I329" s="6"/>
       <c r="J329" s="7"/>
     </row>
-    <row r="330" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="330" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A330" s="4" t="s">
         <v>344</v>
       </c>
@@ -10889,7 +10889,7 @@
       <c r="I330" s="6"/>
       <c r="J330" s="7"/>
     </row>
-    <row r="331" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="331" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A331" s="4" t="s">
         <v>345</v>
       </c>
@@ -10911,7 +10911,7 @@
       <c r="I331" s="6"/>
       <c r="J331" s="7"/>
     </row>
-    <row r="332" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="332" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A332" s="4" t="s">
         <v>346</v>
       </c>
@@ -10933,7 +10933,7 @@
       <c r="I332" s="6"/>
       <c r="J332" s="7"/>
     </row>
-    <row r="333" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="333" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A333" s="4" t="s">
         <v>347</v>
       </c>
@@ -10955,7 +10955,7 @@
       <c r="I333" s="6"/>
       <c r="J333" s="7"/>
     </row>
-    <row r="334" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="334" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A334" s="4" t="s">
         <v>348</v>
       </c>
@@ -10977,7 +10977,7 @@
       <c r="I334" s="6"/>
       <c r="J334" s="7"/>
     </row>
-    <row r="335" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="335" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A335" s="4" t="s">
         <v>349</v>
       </c>
@@ -10999,7 +10999,7 @@
       <c r="I335" s="6"/>
       <c r="J335" s="7"/>
     </row>
-    <row r="336" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="336" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A336" s="4" t="s">
         <v>350</v>
       </c>
@@ -11021,7 +11021,7 @@
       <c r="I336" s="6"/>
       <c r="J336" s="7"/>
     </row>
-    <row r="337" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="337" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A337" s="4" t="s">
         <v>351</v>
       </c>
@@ -11043,7 +11043,7 @@
       <c r="I337" s="6"/>
       <c r="J337" s="7"/>
     </row>
-    <row r="338" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="338" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A338" s="4" t="s">
         <v>352</v>
       </c>
@@ -11065,7 +11065,7 @@
       <c r="I338" s="6"/>
       <c r="J338" s="7"/>
     </row>
-    <row r="339" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="339" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A339" s="4" t="s">
         <v>353</v>
       </c>
@@ -11087,7 +11087,7 @@
       <c r="I339" s="6"/>
       <c r="J339" s="7"/>
     </row>
-    <row r="340" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="340" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A340" s="4" t="s">
         <v>354</v>
       </c>
@@ -11109,7 +11109,7 @@
       <c r="I340" s="6"/>
       <c r="J340" s="7"/>
     </row>
-    <row r="341" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="341" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A341" s="4" t="s">
         <v>355</v>
       </c>
@@ -11131,7 +11131,7 @@
       <c r="I341" s="6"/>
       <c r="J341" s="7"/>
     </row>
-    <row r="342" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="342" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A342" s="4" t="s">
         <v>356</v>
       </c>
@@ -11153,7 +11153,7 @@
       <c r="I342" s="6"/>
       <c r="J342" s="7"/>
     </row>
-    <row r="343" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="343" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A343" s="4" t="s">
         <v>357</v>
       </c>
@@ -11175,7 +11175,7 @@
       <c r="I343" s="6"/>
       <c r="J343" s="7"/>
     </row>
-    <row r="344" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="344" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A344" s="4" t="s">
         <v>358</v>
       </c>
@@ -11197,7 +11197,7 @@
       <c r="I344" s="6"/>
       <c r="J344" s="7"/>
     </row>
-    <row r="345" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="345" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A345" s="4" t="s">
         <v>359</v>
       </c>
@@ -11219,7 +11219,7 @@
       <c r="I345" s="6"/>
       <c r="J345" s="7"/>
     </row>
-    <row r="346" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="346" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A346" s="4" t="s">
         <v>360</v>
       </c>
@@ -11241,7 +11241,7 @@
       <c r="I346" s="6"/>
       <c r="J346" s="7"/>
     </row>
-    <row r="347" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="347" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A347" s="4" t="s">
         <v>361</v>
       </c>
@@ -11263,7 +11263,7 @@
       <c r="I347" s="6"/>
       <c r="J347" s="7"/>
     </row>
-    <row r="348" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="348" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A348" s="4" t="s">
         <v>362</v>
       </c>
@@ -11285,7 +11285,7 @@
       <c r="I348" s="6"/>
       <c r="J348" s="7"/>
     </row>
-    <row r="349" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="349" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A349" s="4" t="s">
         <v>363</v>
       </c>
@@ -11307,7 +11307,7 @@
       <c r="I349" s="6"/>
       <c r="J349" s="7"/>
     </row>
-    <row r="350" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="350" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A350" s="4" t="s">
         <v>364</v>
       </c>
@@ -11329,7 +11329,7 @@
       <c r="I350" s="6"/>
       <c r="J350" s="7"/>
     </row>
-    <row r="351" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="351" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A351" s="4" t="s">
         <v>365</v>
       </c>
@@ -11351,7 +11351,7 @@
       <c r="I351" s="6"/>
       <c r="J351" s="7"/>
     </row>
-    <row r="352" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="352" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A352" s="4" t="s">
         <v>366</v>
       </c>
@@ -11373,7 +11373,7 @@
       <c r="I352" s="6"/>
       <c r="J352" s="7"/>
     </row>
-    <row r="353" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="353" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A353" s="4" t="s">
         <v>367</v>
       </c>
@@ -11395,7 +11395,7 @@
       <c r="I353" s="6"/>
       <c r="J353" s="7"/>
     </row>
-    <row r="354" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="354" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A354" s="4" t="s">
         <v>368</v>
       </c>
@@ -11417,7 +11417,7 @@
       <c r="I354" s="6"/>
       <c r="J354" s="7"/>
     </row>
-    <row r="355" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="355" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A355" s="4" t="s">
         <v>369</v>
       </c>
@@ -11439,7 +11439,7 @@
       <c r="I355" s="6"/>
       <c r="J355" s="7"/>
     </row>
-    <row r="356" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="356" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A356" s="4" t="s">
         <v>370</v>
       </c>
@@ -11461,7 +11461,7 @@
       <c r="I356" s="6"/>
       <c r="J356" s="7"/>
     </row>
-    <row r="357" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="357" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A357" s="4" t="s">
         <v>371</v>
       </c>
@@ -11483,7 +11483,7 @@
       <c r="I357" s="6"/>
       <c r="J357" s="7"/>
     </row>
-    <row r="358" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="358" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A358" s="4" t="s">
         <v>372</v>
       </c>
@@ -11505,7 +11505,7 @@
       <c r="I358" s="6"/>
       <c r="J358" s="7"/>
     </row>
-    <row r="359" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="359" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A359" s="4" t="s">
         <v>373</v>
       </c>
@@ -11527,7 +11527,7 @@
       <c r="I359" s="6"/>
       <c r="J359" s="7"/>
     </row>
-    <row r="360" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="360" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A360" s="9" t="s">
         <v>374</v>
       </c>
@@ -11557,7 +11557,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="361" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="361" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A361" s="4" t="s">
         <v>376</v>
       </c>
@@ -11587,7 +11587,7 @@
         <v>558</v>
       </c>
     </row>
-    <row r="362" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="362" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A362" s="4" t="s">
         <v>377</v>
       </c>
@@ -11617,7 +11617,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="363" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="363" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A363" s="4" t="s">
         <v>378</v>
       </c>
@@ -11647,7 +11647,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="364" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="364" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A364" s="4" t="s">
         <v>379</v>
       </c>
@@ -11677,7 +11677,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="365" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="365" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A365" s="4" t="s">
         <v>380</v>
       </c>
@@ -11707,7 +11707,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="366" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="366" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A366" s="4" t="s">
         <v>381</v>
       </c>
@@ -11737,7 +11737,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="367" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="367" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A367" s="4" t="s">
         <v>382</v>
       </c>
@@ -11767,7 +11767,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="368" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="368" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A368" s="4" t="s">
         <v>383</v>
       </c>
@@ -11797,7 +11797,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="369" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="369" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A369" s="4" t="s">
         <v>384</v>
       </c>
@@ -11827,7 +11827,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="370" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="370" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A370" s="4" t="s">
         <v>385</v>
       </c>
@@ -11857,7 +11857,7 @@
         <v>558</v>
       </c>
     </row>
-    <row r="371" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="371" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A371" s="4" t="s">
         <v>386</v>
       </c>
@@ -11887,7 +11887,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="372" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="372" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A372" s="4" t="s">
         <v>387</v>
       </c>
@@ -11917,7 +11917,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="373" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="373" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A373" s="4" t="s">
         <v>388</v>
       </c>
@@ -11947,7 +11947,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="374" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="374" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A374" s="4" t="s">
         <v>389</v>
       </c>
@@ -11977,7 +11977,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="375" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="375" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A375" s="4" t="s">
         <v>390</v>
       </c>
@@ -12007,7 +12007,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="376" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="376" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A376" s="4" t="s">
         <v>391</v>
       </c>
@@ -12037,7 +12037,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="377" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="377" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A377" s="4" t="s">
         <v>392</v>
       </c>
@@ -12067,7 +12067,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="378" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="378" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A378" s="4" t="s">
         <v>393</v>
       </c>
@@ -12097,7 +12097,7 @@
         <v>558</v>
       </c>
     </row>
-    <row r="379" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="379" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A379" s="4" t="s">
         <v>394</v>
       </c>
@@ -12127,7 +12127,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="380" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="380" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A380" s="4" t="s">
         <v>395</v>
       </c>
@@ -12157,7 +12157,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="381" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="381" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A381" s="4" t="s">
         <v>396</v>
       </c>
@@ -12187,7 +12187,7 @@
         <v>558</v>
       </c>
     </row>
-    <row r="382" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="382" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A382" s="4" t="s">
         <v>397</v>
       </c>
@@ -12217,7 +12217,7 @@
         <v>558</v>
       </c>
     </row>
-    <row r="383" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="383" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A383" s="4" t="s">
         <v>398</v>
       </c>
@@ -12247,7 +12247,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="384" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="384" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A384" s="4" t="s">
         <v>399</v>
       </c>
@@ -12277,7 +12277,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="385" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="385" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A385" s="4" t="s">
         <v>400</v>
       </c>
@@ -12307,7 +12307,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="386" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="386" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A386" s="4" t="s">
         <v>401</v>
       </c>
@@ -12337,7 +12337,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="387" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="387" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A387" s="4" t="s">
         <v>402</v>
       </c>
@@ -12367,7 +12367,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="388" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="388" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A388" s="4" t="s">
         <v>403</v>
       </c>
@@ -12397,7 +12397,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="389" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="389" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A389" s="4" t="s">
         <v>404</v>
       </c>
@@ -12427,7 +12427,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="390" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="390" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A390" s="4" t="s">
         <v>405</v>
       </c>
@@ -12457,7 +12457,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="391" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="391" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A391" s="4" t="s">
         <v>406</v>
       </c>
@@ -12487,7 +12487,7 @@
         <v>543</v>
       </c>
     </row>
-    <row r="392" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="392" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A392" s="4" t="s">
         <v>407</v>
       </c>
@@ -12517,7 +12517,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="393" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="393" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A393" s="4" t="s">
         <v>408</v>
       </c>
@@ -12547,7 +12547,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="394" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="394" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A394" s="4" t="s">
         <v>409</v>
       </c>
@@ -12577,7 +12577,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="395" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="395" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A395" s="4" t="s">
         <v>410</v>
       </c>
@@ -12607,7 +12607,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="396" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="396" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A396" s="4" t="s">
         <v>411</v>
       </c>
@@ -12637,7 +12637,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="397" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="397" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A397" s="4" t="s">
         <v>412</v>
       </c>
@@ -12667,7 +12667,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="398" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="398" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A398" s="4" t="s">
         <v>413</v>
       </c>
@@ -12697,7 +12697,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="399" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="399" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A399" s="4" t="s">
         <v>414</v>
       </c>
@@ -12727,7 +12727,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="400" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="400" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A400" s="4" t="s">
         <v>415</v>
       </c>
@@ -12757,7 +12757,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="401" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="401" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A401" s="4" t="s">
         <v>416</v>
       </c>
@@ -12787,7 +12787,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="402" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="402" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A402" s="4" t="s">
         <v>417</v>
       </c>
@@ -12817,7 +12817,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="403" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="403" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A403" s="4" t="s">
         <v>418</v>
       </c>
@@ -12847,7 +12847,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="404" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="404" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A404" s="4" t="s">
         <v>419</v>
       </c>
@@ -12877,7 +12877,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="405" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="405" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A405" s="4" t="s">
         <v>420</v>
       </c>
@@ -12907,7 +12907,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="406" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="406" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A406" s="4" t="s">
         <v>421</v>
       </c>
@@ -12937,7 +12937,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="407" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="407" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A407" s="4" t="s">
         <v>422</v>
       </c>
@@ -12967,7 +12967,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="408" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="408" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A408" s="4" t="s">
         <v>423</v>
       </c>
@@ -12997,7 +12997,7 @@
         <v>558</v>
       </c>
     </row>
-    <row r="409" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="409" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A409" s="4" t="s">
         <v>424</v>
       </c>
@@ -13027,7 +13027,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="410" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="410" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A410" s="4" t="s">
         <v>425</v>
       </c>
@@ -13049,7 +13049,7 @@
       <c r="I410" s="8"/>
       <c r="J410" s="18"/>
     </row>
-    <row r="411" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="411" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A411" s="4" t="s">
         <v>426</v>
       </c>
@@ -13071,7 +13071,7 @@
       <c r="I411" s="8"/>
       <c r="J411" s="18"/>
     </row>
-    <row r="412" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="412" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A412" s="4" t="s">
         <v>427</v>
       </c>
@@ -13093,7 +13093,7 @@
       <c r="I412" s="8"/>
       <c r="J412" s="18"/>
     </row>
-    <row r="413" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="413" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A413" s="4" t="s">
         <v>428</v>
       </c>
@@ -13115,7 +13115,7 @@
       <c r="I413" s="8"/>
       <c r="J413" s="18"/>
     </row>
-    <row r="414" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="414" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A414" s="4" t="s">
         <v>429</v>
       </c>
@@ -13137,7 +13137,7 @@
       <c r="I414" s="8"/>
       <c r="J414" s="18"/>
     </row>
-    <row r="415" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="415" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A415" s="4" t="s">
         <v>430</v>
       </c>
@@ -13159,7 +13159,7 @@
       <c r="I415" s="8"/>
       <c r="J415" s="18"/>
     </row>
-    <row r="416" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="416" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A416" s="4" t="s">
         <v>431</v>
       </c>
@@ -13181,7 +13181,7 @@
       <c r="I416" s="8"/>
       <c r="J416" s="18"/>
     </row>
-    <row r="417" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="417" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A417" s="4" t="s">
         <v>432</v>
       </c>
@@ -13203,7 +13203,7 @@
       <c r="I417" s="8"/>
       <c r="J417" s="18"/>
     </row>
-    <row r="418" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="418" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A418" s="4" t="s">
         <v>433</v>
       </c>
@@ -13225,7 +13225,7 @@
       <c r="I418" s="8"/>
       <c r="J418" s="18"/>
     </row>
-    <row r="419" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="419" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A419" s="4" t="s">
         <v>434</v>
       </c>
@@ -13247,7 +13247,7 @@
       <c r="I419" s="8"/>
       <c r="J419" s="18"/>
     </row>
-    <row r="420" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="420" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A420" s="4" t="s">
         <v>435</v>
       </c>
@@ -13269,7 +13269,7 @@
       <c r="I420" s="8"/>
       <c r="J420" s="18"/>
     </row>
-    <row r="421" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="421" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A421" s="4" t="s">
         <v>436</v>
       </c>
@@ -13291,7 +13291,7 @@
       <c r="I421" s="8"/>
       <c r="J421" s="18"/>
     </row>
-    <row r="422" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="422" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A422" s="4" t="s">
         <v>437</v>
       </c>
@@ -13313,7 +13313,7 @@
       <c r="I422" s="8"/>
       <c r="J422" s="18"/>
     </row>
-    <row r="423" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="423" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A423" s="4" t="s">
         <v>438</v>
       </c>
@@ -13335,7 +13335,7 @@
       <c r="I423" s="8"/>
       <c r="J423" s="18"/>
     </row>
-    <row r="424" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="424" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A424" s="4" t="s">
         <v>439</v>
       </c>
@@ -13357,7 +13357,7 @@
       <c r="I424" s="8"/>
       <c r="J424" s="18"/>
     </row>
-    <row r="425" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="425" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A425" s="4" t="s">
         <v>440</v>
       </c>
@@ -13379,7 +13379,7 @@
       <c r="I425" s="8"/>
       <c r="J425" s="18"/>
     </row>
-    <row r="426" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="426" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A426" s="4" t="s">
         <v>441</v>
       </c>
@@ -13401,7 +13401,7 @@
       <c r="I426" s="8"/>
       <c r="J426" s="18"/>
     </row>
-    <row r="427" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="427" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A427" s="4" t="s">
         <v>442</v>
       </c>
@@ -13423,7 +13423,7 @@
       <c r="I427" s="8"/>
       <c r="J427" s="18"/>
     </row>
-    <row r="428" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="428" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A428" s="4" t="s">
         <v>443</v>
       </c>
@@ -13445,7 +13445,7 @@
       <c r="I428" s="8"/>
       <c r="J428" s="18"/>
     </row>
-    <row r="429" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="429" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A429" s="4" t="s">
         <v>444</v>
       </c>
@@ -13467,7 +13467,7 @@
       <c r="I429" s="8"/>
       <c r="J429" s="18"/>
     </row>
-    <row r="430" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="430" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A430" s="4" t="s">
         <v>445</v>
       </c>
@@ -13489,7 +13489,7 @@
       <c r="I430" s="8"/>
       <c r="J430" s="18"/>
     </row>
-    <row r="431" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="431" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A431" s="4" t="s">
         <v>446</v>
       </c>
@@ -13511,7 +13511,7 @@
       <c r="I431" s="8"/>
       <c r="J431" s="18"/>
     </row>
-    <row r="432" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="432" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A432" s="4" t="s">
         <v>447</v>
       </c>
@@ -13533,7 +13533,7 @@
       <c r="I432" s="8"/>
       <c r="J432" s="18"/>
     </row>
-    <row r="433" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="433" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A433" s="4" t="s">
         <v>448</v>
       </c>
@@ -13555,7 +13555,7 @@
       <c r="I433" s="8"/>
       <c r="J433" s="18"/>
     </row>
-    <row r="434" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="434" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A434" s="4" t="s">
         <v>449</v>
       </c>
@@ -13577,7 +13577,7 @@
       <c r="I434" s="8"/>
       <c r="J434" s="18"/>
     </row>
-    <row r="435" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="435" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A435" s="4" t="s">
         <v>450</v>
       </c>
@@ -13599,7 +13599,7 @@
       <c r="I435" s="8"/>
       <c r="J435" s="18"/>
     </row>
-    <row r="436" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="436" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A436" s="4" t="s">
         <v>451</v>
       </c>
@@ -13621,7 +13621,7 @@
       <c r="I436" s="8"/>
       <c r="J436" s="18"/>
     </row>
-    <row r="437" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="437" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A437" s="4" t="s">
         <v>452</v>
       </c>
@@ -13643,7 +13643,7 @@
       <c r="I437" s="8"/>
       <c r="J437" s="18"/>
     </row>
-    <row r="438" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="438" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A438" s="4" t="s">
         <v>453</v>
       </c>
@@ -13665,7 +13665,7 @@
       <c r="I438" s="8"/>
       <c r="J438" s="18"/>
     </row>
-    <row r="439" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="439" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A439" s="4" t="s">
         <v>454</v>
       </c>
@@ -13687,7 +13687,7 @@
       <c r="I439" s="8"/>
       <c r="J439" s="18"/>
     </row>
-    <row r="440" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="440" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A440" s="4" t="s">
         <v>455</v>
       </c>
@@ -13709,7 +13709,7 @@
       <c r="I440" s="8"/>
       <c r="J440" s="18"/>
     </row>
-    <row r="441" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="441" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A441" s="4" t="s">
         <v>456</v>
       </c>
@@ -13731,7 +13731,7 @@
       <c r="I441" s="8"/>
       <c r="J441" s="18"/>
     </row>
-    <row r="442" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="442" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A442" s="4" t="s">
         <v>457</v>
       </c>
@@ -13753,7 +13753,7 @@
       <c r="I442" s="6"/>
       <c r="J442" s="18"/>
     </row>
-    <row r="443" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="443" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A443" s="4" t="s">
         <v>458</v>
       </c>
@@ -13775,7 +13775,7 @@
       <c r="I443" s="6"/>
       <c r="J443" s="18"/>
     </row>
-    <row r="444" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="444" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A444" s="4" t="s">
         <v>459</v>
       </c>
@@ -13797,7 +13797,7 @@
       <c r="I444" s="6"/>
       <c r="J444" s="18"/>
     </row>
-    <row r="445" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="445" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A445" s="4" t="s">
         <v>460</v>
       </c>
@@ -13819,7 +13819,7 @@
       <c r="I445" s="6"/>
       <c r="J445" s="18"/>
     </row>
-    <row r="446" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="446" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A446" s="4" t="s">
         <v>461</v>
       </c>
@@ -13841,7 +13841,7 @@
       <c r="I446" s="6"/>
       <c r="J446" s="18"/>
     </row>
-    <row r="447" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="447" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A447" s="4" t="s">
         <v>462</v>
       </c>
@@ -13863,7 +13863,7 @@
       <c r="I447" s="6"/>
       <c r="J447" s="18"/>
     </row>
-    <row r="448" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="448" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A448" s="4" t="s">
         <v>463</v>
       </c>
@@ -13885,7 +13885,7 @@
       <c r="I448" s="6"/>
       <c r="J448" s="18"/>
     </row>
-    <row r="449" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="449" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A449" s="4" t="s">
         <v>464</v>
       </c>
@@ -13907,7 +13907,7 @@
       <c r="I449" s="6"/>
       <c r="J449" s="18"/>
     </row>
-    <row r="450" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="450" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A450" s="4" t="s">
         <v>465</v>
       </c>
@@ -13929,7 +13929,7 @@
       <c r="I450" s="6"/>
       <c r="J450" s="18"/>
     </row>
-    <row r="451" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="451" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A451" s="4" t="s">
         <v>466</v>
       </c>
@@ -13951,7 +13951,7 @@
       <c r="I451" s="6"/>
       <c r="J451" s="18"/>
     </row>
-    <row r="452" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="452" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A452" s="4" t="s">
         <v>467</v>
       </c>
@@ -13973,7 +13973,7 @@
       <c r="I452" s="6"/>
       <c r="J452" s="18"/>
     </row>
-    <row r="453" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="453" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A453" s="4" t="s">
         <v>468</v>
       </c>
@@ -13995,7 +13995,7 @@
       <c r="I453" s="6"/>
       <c r="J453" s="18"/>
     </row>
-    <row r="454" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="454" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A454" s="4" t="s">
         <v>469</v>
       </c>
@@ -14017,7 +14017,7 @@
       <c r="I454" s="6"/>
       <c r="J454" s="18"/>
     </row>
-    <row r="455" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="455" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A455" s="4" t="s">
         <v>470</v>
       </c>
@@ -14039,7 +14039,7 @@
       <c r="I455" s="6"/>
       <c r="J455" s="18"/>
     </row>
-    <row r="456" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="456" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A456" s="4" t="s">
         <v>471</v>
       </c>
@@ -14061,7 +14061,7 @@
       <c r="I456" s="6"/>
       <c r="J456" s="18"/>
     </row>
-    <row r="457" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="457" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A457" s="4" t="s">
         <v>472</v>
       </c>
@@ -14083,7 +14083,7 @@
       <c r="I457" s="6"/>
       <c r="J457" s="18"/>
     </row>
-    <row r="458" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="458" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A458" s="4" t="s">
         <v>473</v>
       </c>
@@ -14105,7 +14105,7 @@
       <c r="I458" s="6"/>
       <c r="J458" s="18"/>
     </row>
-    <row r="459" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="459" spans="1:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A459" s="13" t="s">
         <v>474</v>
       </c>
@@ -14127,7 +14127,7 @@
       <c r="I459" s="15"/>
       <c r="J459" s="20"/>
     </row>
-    <row r="460" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="460" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A460" s="4" t="s">
         <v>475</v>
       </c>
@@ -14149,7 +14149,7 @@
       <c r="I460" s="6"/>
       <c r="J460" s="18"/>
     </row>
-    <row r="461" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="461" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A461" s="4" t="s">
         <v>477</v>
       </c>
@@ -14171,7 +14171,7 @@
       <c r="I461" s="6"/>
       <c r="J461" s="18"/>
     </row>
-    <row r="462" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="462" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A462" s="4" t="s">
         <v>478</v>
       </c>
@@ -14193,7 +14193,7 @@
       <c r="I462" s="6"/>
       <c r="J462" s="18"/>
     </row>
-    <row r="463" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="463" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A463" s="4" t="s">
         <v>479</v>
       </c>
@@ -14215,7 +14215,7 @@
       <c r="I463" s="6"/>
       <c r="J463" s="18"/>
     </row>
-    <row r="464" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="464" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A464" s="4" t="s">
         <v>480</v>
       </c>
@@ -14237,7 +14237,7 @@
       <c r="I464" s="6"/>
       <c r="J464" s="18"/>
     </row>
-    <row r="465" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="465" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A465" s="4" t="s">
         <v>481</v>
       </c>
@@ -14259,7 +14259,7 @@
       <c r="I465" s="6"/>
       <c r="J465" s="18"/>
     </row>
-    <row r="466" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="466" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A466" s="4" t="s">
         <v>482</v>
       </c>
@@ -14281,7 +14281,7 @@
       <c r="I466" s="6"/>
       <c r="J466" s="18"/>
     </row>
-    <row r="467" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="467" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A467" s="4" t="s">
         <v>483</v>
       </c>
@@ -14303,7 +14303,7 @@
       <c r="I467" s="21"/>
       <c r="J467" s="18"/>
     </row>
-    <row r="468" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="468" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A468" s="4" t="s">
         <v>484</v>
       </c>
@@ -14325,7 +14325,7 @@
       <c r="I468" s="6"/>
       <c r="J468" s="22"/>
     </row>
-    <row r="469" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="469" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A469" s="4" t="s">
         <v>485</v>
       </c>
@@ -14347,7 +14347,7 @@
       <c r="I469" s="6"/>
       <c r="J469" s="18"/>
     </row>
-    <row r="470" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="470" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A470" s="4" t="s">
         <v>486</v>
       </c>
@@ -14369,7 +14369,7 @@
       <c r="I470" s="6"/>
       <c r="J470" s="18"/>
     </row>
-    <row r="471" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="471" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A471" s="4" t="s">
         <v>487</v>
       </c>
@@ -14391,7 +14391,7 @@
       <c r="I471" s="6"/>
       <c r="J471" s="18"/>
     </row>
-    <row r="472" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="472" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A472" s="23" t="s">
         <v>488</v>
       </c>
@@ -14413,7 +14413,7 @@
       <c r="I472" s="25"/>
       <c r="J472" s="26"/>
     </row>
-    <row r="473" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="473" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A473" s="23" t="s">
         <v>489</v>
       </c>
@@ -14435,7 +14435,7 @@
       <c r="I473" s="25"/>
       <c r="J473" s="26"/>
     </row>
-    <row r="474" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="474" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A474" s="23" t="s">
         <v>490</v>
       </c>
@@ -14457,7 +14457,7 @@
       <c r="I474" s="25"/>
       <c r="J474" s="26"/>
     </row>
-    <row r="475" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="475" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A475" s="23" t="s">
         <v>491</v>
       </c>
@@ -14479,7 +14479,7 @@
       <c r="I475" s="25"/>
       <c r="J475" s="26"/>
     </row>
-    <row r="476" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="476" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A476" s="23" t="s">
         <v>492</v>
       </c>
@@ -14501,7 +14501,7 @@
       <c r="I476" s="25"/>
       <c r="J476" s="26"/>
     </row>
-    <row r="477" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="477" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A477" s="23" t="s">
         <v>493</v>
       </c>
@@ -14523,7 +14523,7 @@
       <c r="I477" s="25"/>
       <c r="J477" s="26"/>
     </row>
-    <row r="478" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="478" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A478" s="23" t="s">
         <v>494</v>
       </c>
@@ -14545,7 +14545,7 @@
       <c r="I478" s="25"/>
       <c r="J478" s="26"/>
     </row>
-    <row r="479" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="479" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A479" s="23" t="s">
         <v>495</v>
       </c>
@@ -14567,7 +14567,7 @@
       <c r="I479" s="25"/>
       <c r="J479" s="26"/>
     </row>
-    <row r="480" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="480" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A480" s="23" t="s">
         <v>496</v>
       </c>
@@ -14591,7 +14591,7 @@
       </c>
       <c r="J480" s="26"/>
     </row>
-    <row r="481" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="481" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A481" s="23" t="s">
         <v>497</v>
       </c>
@@ -14615,7 +14615,7 @@
       </c>
       <c r="J481" s="26"/>
     </row>
-    <row r="482" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="482" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A482" s="23" t="s">
         <v>498</v>
       </c>
@@ -14639,7 +14639,7 @@
       </c>
       <c r="J482" s="26"/>
     </row>
-    <row r="483" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="483" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A483" s="23" t="s">
         <v>499</v>
       </c>
@@ -14663,7 +14663,7 @@
       </c>
       <c r="J483" s="26"/>
     </row>
-    <row r="484" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="484" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A484" s="23" t="s">
         <v>500</v>
       </c>
@@ -14687,7 +14687,7 @@
       </c>
       <c r="J484" s="26"/>
     </row>
-    <row r="485" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="485" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A485" s="23" t="s">
         <v>501</v>
       </c>
@@ -14711,7 +14711,7 @@
       </c>
       <c r="J485" s="26"/>
     </row>
-    <row r="486" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="486" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A486" s="23" t="s">
         <v>502</v>
       </c>
@@ -14735,7 +14735,7 @@
       </c>
       <c r="J486" s="26"/>
     </row>
-    <row r="487" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="487" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A487" s="23" t="s">
         <v>503</v>
       </c>
@@ -14759,7 +14759,7 @@
       </c>
       <c r="J487" s="26"/>
     </row>
-    <row r="488" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="488" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A488" s="23" t="s">
         <v>504</v>
       </c>
@@ -14783,7 +14783,7 @@
       </c>
       <c r="J488" s="26"/>
     </row>
-    <row r="489" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="489" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A489" s="23" t="s">
         <v>505</v>
       </c>
@@ -14807,7 +14807,7 @@
       </c>
       <c r="J489" s="26"/>
     </row>
-    <row r="490" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="490" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A490" s="23" t="s">
         <v>506</v>
       </c>
@@ -14831,7 +14831,7 @@
       </c>
       <c r="J490" s="26"/>
     </row>
-    <row r="491" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="491" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A491" s="23" t="s">
         <v>507</v>
       </c>
@@ -14855,7 +14855,7 @@
       </c>
       <c r="J491" s="26"/>
     </row>
-    <row r="492" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="492" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A492" s="23" t="s">
         <v>508</v>
       </c>
@@ -14879,7 +14879,7 @@
       </c>
       <c r="J492" s="26"/>
     </row>
-    <row r="493" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="493" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A493" s="23" t="s">
         <v>509</v>
       </c>
@@ -14901,7 +14901,7 @@
       <c r="I493" s="25"/>
       <c r="J493" s="26"/>
     </row>
-    <row r="494" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="494" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A494" s="23" t="s">
         <v>510</v>
       </c>
@@ -14925,7 +14925,7 @@
       </c>
       <c r="J494" s="26"/>
     </row>
-    <row r="495" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="495" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A495" s="23" t="s">
         <v>511</v>
       </c>
@@ -14949,7 +14949,7 @@
       </c>
       <c r="J495" s="26"/>
     </row>
-    <row r="496" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="496" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A496" s="23" t="s">
         <v>512</v>
       </c>
@@ -14973,7 +14973,7 @@
       </c>
       <c r="J496" s="26"/>
     </row>
-    <row r="497" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="497" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A497" s="23" t="s">
         <v>513</v>
       </c>
@@ -14997,7 +14997,7 @@
       </c>
       <c r="J497" s="26"/>
     </row>
-    <row r="498" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="498" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A498" s="23" t="s">
         <v>514</v>
       </c>
@@ -15021,7 +15021,7 @@
       </c>
       <c r="J498" s="26"/>
     </row>
-    <row r="499" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="499" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A499" s="23" t="s">
         <v>515</v>
       </c>
@@ -15045,7 +15045,7 @@
       </c>
       <c r="J499" s="26"/>
     </row>
-    <row r="500" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="500" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A500" s="23" t="s">
         <v>516</v>
       </c>
@@ -15069,7 +15069,7 @@
       </c>
       <c r="J500" s="26"/>
     </row>
-    <row r="501" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="501" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A501" s="23" t="s">
         <v>517</v>
       </c>
@@ -15093,7 +15093,7 @@
       </c>
       <c r="J501" s="26"/>
     </row>
-    <row r="502" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="502" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A502" s="23" t="s">
         <v>518</v>
       </c>
@@ -15117,7 +15117,7 @@
       </c>
       <c r="J502" s="26"/>
     </row>
-    <row r="503" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="503" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A503" s="23" t="s">
         <v>519</v>
       </c>
@@ -15141,7 +15141,7 @@
       </c>
       <c r="J503" s="26"/>
     </row>
-    <row r="504" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="504" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A504" s="23" t="s">
         <v>520</v>
       </c>
@@ -15165,7 +15165,7 @@
       </c>
       <c r="J504" s="26"/>
     </row>
-    <row r="505" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="505" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A505" s="23" t="s">
         <v>521</v>
       </c>
@@ -15189,7 +15189,7 @@
       </c>
       <c r="J505" s="26"/>
     </row>
-    <row r="506" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="506" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A506" s="23" t="s">
         <v>522</v>
       </c>
@@ -15213,7 +15213,7 @@
       </c>
       <c r="J506" s="26"/>
     </row>
-    <row r="507" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="507" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A507" s="27" t="s">
         <v>523</v>
       </c>
@@ -15237,7 +15237,7 @@
       </c>
       <c r="J507" s="30"/>
     </row>
-    <row r="508" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="508" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A508" s="24"/>
       <c r="B508" s="24"/>
       <c r="C508" s="24"/>
@@ -15249,7 +15249,7 @@
       <c r="I508" s="24"/>
       <c r="J508" s="24"/>
     </row>
-    <row r="509" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="509" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A509" s="24"/>
       <c r="B509" s="24"/>
       <c r="C509" s="24"/>
@@ -15261,7 +15261,7 @@
       <c r="I509" s="24"/>
       <c r="J509" s="24"/>
     </row>
-    <row r="510" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="510" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A510" s="24"/>
       <c r="B510" s="24"/>
       <c r="C510" s="24"/>
@@ -15273,7 +15273,7 @@
       <c r="I510" s="24"/>
       <c r="J510" s="24"/>
     </row>
-    <row r="511" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="511" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A511" s="24"/>
       <c r="B511" s="24"/>
       <c r="C511" s="24"/>
@@ -15285,7 +15285,7 @@
       <c r="I511" s="24"/>
       <c r="J511" s="24"/>
     </row>
-    <row r="512" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="512" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A512" s="24"/>
       <c r="B512" s="24"/>
       <c r="C512" s="24"/>
@@ -15297,7 +15297,7 @@
       <c r="I512" s="24"/>
       <c r="J512" s="24"/>
     </row>
-    <row r="513" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="513" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A513" s="24"/>
       <c r="B513" s="24"/>
       <c r="C513" s="24"/>
@@ -15309,7 +15309,7 @@
       <c r="I513" s="24"/>
       <c r="J513" s="24"/>
     </row>
-    <row r="514" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="514" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A514" s="24"/>
       <c r="B514" s="24"/>
       <c r="C514" s="24"/>
@@ -15321,7 +15321,7 @@
       <c r="I514" s="24"/>
       <c r="J514" s="24"/>
     </row>
-    <row r="515" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="515" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A515" s="24"/>
       <c r="B515" s="24"/>
       <c r="C515" s="24"/>
@@ -15333,7 +15333,7 @@
       <c r="I515" s="24"/>
       <c r="J515" s="24"/>
     </row>
-    <row r="516" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="516" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A516" s="24"/>
       <c r="B516" s="24"/>
       <c r="C516" s="24"/>
@@ -15345,7 +15345,7 @@
       <c r="I516" s="24"/>
       <c r="J516" s="24"/>
     </row>
-    <row r="517" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="517" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A517" s="24"/>
       <c r="B517" s="24"/>
       <c r="C517" s="24"/>
@@ -15357,7 +15357,7 @@
       <c r="I517" s="24"/>
       <c r="J517" s="24"/>
     </row>
-    <row r="518" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="518" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A518" s="24"/>
       <c r="B518" s="24"/>
       <c r="C518" s="24"/>
@@ -15369,7 +15369,7 @@
       <c r="I518" s="24"/>
       <c r="J518" s="24"/>
     </row>
-    <row r="519" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="519" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A519" s="24"/>
       <c r="B519" s="24"/>
       <c r="C519" s="24"/>
@@ -15381,7 +15381,7 @@
       <c r="I519" s="24"/>
       <c r="J519" s="24"/>
     </row>
-    <row r="520" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="520" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A520" s="24"/>
       <c r="B520" s="24"/>
       <c r="C520" s="24"/>
@@ -15395,5 +15395,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>